<commit_message>
Removed drug cohorts from O in Analysis 1
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis1.xlsx
+++ b/analysis_specifications/analysis1.xlsx
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C366"/>
+  <dimension ref="A1:C330"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4247,11 +4247,11 @@
     </row>
     <row r="297">
       <c r="A297">
-        <v>1035</v>
+        <v>1072</v>
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>New users of Thiazide diuretics</t>
+          <t>Cytomegalovirus CMV Anterior Uveitis</t>
         </is>
       </c>
       <c r="C297">
@@ -4260,258 +4260,258 @@
     </row>
     <row r="298">
       <c r="A298">
-        <v>1036</v>
+        <v>1073</v>
       </c>
       <c r="B298" t="inlineStr">
         <is>
-          <t>New users of Beta blockers</t>
+          <t>Serious Infection, opportunistic infections and other infections of interest event</t>
         </is>
       </c>
       <c r="C298">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="299">
       <c r="A299">
-        <v>1037</v>
+        <v>1074</v>
       </c>
       <c r="B299" t="inlineStr">
         <is>
-          <t>New users of SGLT2 inhibitor</t>
+          <t>Serious Infection</t>
         </is>
       </c>
       <c r="C299">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="300">
       <c r="A300">
-        <v>1038</v>
+        <v>1075</v>
       </c>
       <c r="B300" t="inlineStr">
         <is>
-          <t>New users of GLP-1 receptor antagonists</t>
+          <t>Narcolepsy</t>
         </is>
       </c>
       <c r="C300">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="301">
       <c r="A301">
-        <v>1039</v>
+        <v>1076</v>
       </c>
       <c r="B301" t="inlineStr">
         <is>
-          <t>New users of DPP-4 inhibitors</t>
+          <t>Anaphylaxis</t>
         </is>
       </c>
       <c r="C301">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="302">
       <c r="A302">
-        <v>1040</v>
+        <v>1077</v>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>New users of Tumor Necrosis Factor alpha (TNFa) inhibitors</t>
+          <t>Anaphylaxis v2</t>
         </is>
       </c>
       <c r="C302">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="303">
       <c r="A303">
-        <v>1041</v>
+        <v>1078</v>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>New users of JAK inhibitors</t>
+          <t>Bells Palsy</t>
         </is>
       </c>
       <c r="C303">
-        <v>0</v>
+        <v>183</v>
       </c>
     </row>
     <row r="304">
       <c r="A304">
-        <v>1042</v>
+        <v>1079</v>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>New users of IL-23 inhibitors</t>
+          <t>Encephalomyelitis</t>
         </is>
       </c>
       <c r="C304">
-        <v>0</v>
+        <v>183</v>
       </c>
     </row>
     <row r="305">
       <c r="A305">
-        <v>1043</v>
+        <v>1080</v>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>New users of Fluoroquinolone systemic</t>
+          <t>Guillain Barre Syndrome</t>
         </is>
       </c>
       <c r="C305">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="306">
       <c r="A306">
-        <v>1044</v>
+        <v>1081</v>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>New users of Cephalosporin systemetic</t>
+          <t>Acute Myocardial Infarction including its complications</t>
         </is>
       </c>
       <c r="C306">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="307">
       <c r="A307">
-        <v>1045</v>
+        <v>1082</v>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>New users of Trimethoprim systemetic</t>
+          <t>Myocarditis Pericarditis</t>
         </is>
       </c>
       <c r="C307">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="308">
       <c r="A308">
-        <v>1046</v>
+        <v>1083</v>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>New users of Thiazide diuretics nested in essential hypertension</t>
+          <t>Immune Thrombocytopenia (ITP)</t>
         </is>
       </c>
       <c r="C308">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="309">
       <c r="A309">
-        <v>1047</v>
+        <v>1084</v>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>New users of dihydropyridine calcium channel blockers nested in essential hypertension</t>
+          <t>Disseminated Intravascular Coagulation</t>
         </is>
       </c>
       <c r="C309">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="310">
       <c r="A310">
-        <v>1048</v>
+        <v>1085</v>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>New users of dihydropyridine calcium channel blockers</t>
+          <t>Appendicitis</t>
         </is>
       </c>
       <c r="C310">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="311">
       <c r="A311">
-        <v>1049</v>
+        <v>1086</v>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>New users of Beta blockers nested in essential hypertension</t>
+          <t>Transverse Myelitis</t>
         </is>
       </c>
       <c r="C311">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="312">
       <c r="A312">
-        <v>1050</v>
+        <v>1087</v>
       </c>
       <c r="B312" t="inlineStr">
         <is>
-          <t>New users of Beta blockers nested in Left Heart Failure</t>
+          <t>Hemorrhagic Stroke</t>
         </is>
       </c>
       <c r="C312">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="313">
       <c r="A313">
-        <v>1051</v>
+        <v>1088</v>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>New users of SGLT2 inhibitor nested in Left Heart Failure</t>
+          <t>Deep Vein Thrombosis (DVT)</t>
         </is>
       </c>
       <c r="C313">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="314">
       <c r="A314">
-        <v>1052</v>
+        <v>1089</v>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>New users of Beta blockers nested in Acute Myocardial Infarction</t>
+          <t>Non-hemorrhagic Stroke</t>
         </is>
       </c>
       <c r="C314">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="315">
       <c r="A315">
-        <v>1053</v>
+        <v>1090</v>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>New users of GLP-1 receptor antagonists nested in Type 2 diabetes mellitus</t>
+          <t>Pulmonary Embolism</t>
         </is>
       </c>
       <c r="C315">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="316">
       <c r="A316">
-        <v>1054</v>
+        <v>1091</v>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>New users of SGLT2 inhibitor nested in Type 2 diabetes mellitus</t>
+          <t>Thrombosis with Thrombocytopenia (TWT)</t>
         </is>
       </c>
       <c r="C316">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="317">
       <c r="A317">
-        <v>1055</v>
+        <v>1093</v>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>New users of DPP-4 inhibitors nested in Type 2 diabetes mellitus</t>
+          <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C317">
@@ -4520,11 +4520,11 @@
     </row>
     <row r="318">
       <c r="A318">
-        <v>1056</v>
+        <v>1094</v>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>New users of GLP-1 receptor antagonists nested in obesity</t>
+          <t>Lower Extremity Bypass - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C318">
@@ -4533,11 +4533,11 @@
     </row>
     <row r="319">
       <c r="A319">
-        <v>1057</v>
+        <v>1095</v>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>New users of IL-23 inhibitors nested in Plaque psoriasis</t>
+          <t>Carotid Endarterectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C319">
@@ -4546,11 +4546,11 @@
     </row>
     <row r="320">
       <c r="A320">
-        <v>1058</v>
+        <v>1096</v>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>New users of Tumor Necrosis Factor alpha (TNFa) inhibitors nested in Plaque psoriasis</t>
+          <t>Lung Resection - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C320">
@@ -4559,11 +4559,11 @@
     </row>
     <row r="321">
       <c r="A321">
-        <v>1059</v>
+        <v>1097</v>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>New users of Tumor Necrosis Factor alpha (TNFa) inhibitors nested in Psoriatic Arthritis</t>
+          <t>Esophagectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C321">
@@ -4572,11 +4572,11 @@
     </row>
     <row r="322">
       <c r="A322">
-        <v>1060</v>
+        <v>1098</v>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>New users of Fluoroquinolone systemic nested in Urinary Tract Infection</t>
+          <t>Pancreatectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C322">
@@ -4585,11 +4585,11 @@
     </row>
     <row r="323">
       <c r="A323">
-        <v>1061</v>
+        <v>1099</v>
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>New users of Cephalosporin systemetic nested in Urinary Tract Infection</t>
+          <t>Colectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C323">
@@ -4598,11 +4598,11 @@
     </row>
     <row r="324">
       <c r="A324">
-        <v>1062</v>
+        <v>1100</v>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>New users of Trimethoprim systemetic nested in Urinary Tract Infection</t>
+          <t>Cystectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C324">
@@ -4611,11 +4611,11 @@
     </row>
     <row r="325">
       <c r="A325">
-        <v>1063</v>
+        <v>1101</v>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>New users of Fluoroquinolone systemic nested in Acute Typical Pneumonia</t>
+          <t>Nephrectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C325">
@@ -4624,11 +4624,11 @@
     </row>
     <row r="326">
       <c r="A326">
-        <v>1064</v>
+        <v>1102</v>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>New users of Cephalosporin systemetic nested in Acute Typical Pneumonia</t>
+          <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C326">
@@ -4637,11 +4637,11 @@
     </row>
     <row r="327">
       <c r="A327">
-        <v>1065</v>
+        <v>1103</v>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>New users of Trimethoprim systemetic nested in Acute Typical Pneumonia</t>
+          <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C327">
@@ -4650,11 +4650,11 @@
     </row>
     <row r="328">
       <c r="A328">
-        <v>1066</v>
+        <v>1104</v>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>New users of Tumor Necrosis Factor alpha (TNFa) inhibitors nested in Rheumatoid arthritis</t>
+          <t>RBC Transfusion (adult relevant, no auto 1yr clean window)</t>
         </is>
       </c>
       <c r="C328">
@@ -4663,11 +4663,11 @@
     </row>
     <row r="329">
       <c r="A329">
-        <v>1067</v>
+        <v>1105</v>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>New users of JAK inhibitors nested in Ulcerative colitis</t>
+          <t>Clostridium difficile - first episode</t>
         </is>
       </c>
       <c r="C329">
@@ -4676,482 +4676,14 @@
     </row>
     <row r="330">
       <c r="A330">
-        <v>1068</v>
+        <v>1106</v>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>New users of Tumor Necrosis Factor alpha (TNFa) inhibitors nested in Ulcerative colitis</t>
+          <t>Non-Emergent Major Non Cardiac Surgery no prior Opioid</t>
         </is>
       </c>
       <c r="C330">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="331">
-      <c r="A331">
-        <v>1069</v>
-      </c>
-      <c r="B331" t="inlineStr">
-        <is>
-          <t>New users of Tumor Necrosis Factor alpha (TNFa) inhibitors nested in Crohns disease</t>
-        </is>
-      </c>
-      <c r="C331">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="332">
-      <c r="A332">
-        <v>1070</v>
-      </c>
-      <c r="B332" t="inlineStr">
-        <is>
-          <t>New users of JAK inhibitors nested in Rheumatoid arthritis</t>
-        </is>
-      </c>
-      <c r="C332">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="333">
-      <c r="A333">
-        <v>1072</v>
-      </c>
-      <c r="B333" t="inlineStr">
-        <is>
-          <t>Cytomegalovirus CMV Anterior Uveitis</t>
-        </is>
-      </c>
-      <c r="C333">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="334">
-      <c r="A334">
-        <v>1073</v>
-      </c>
-      <c r="B334" t="inlineStr">
-        <is>
-          <t>Serious Infection, opportunistic infections and other infections of interest event</t>
-        </is>
-      </c>
-      <c r="C334">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="335">
-      <c r="A335">
-        <v>1074</v>
-      </c>
-      <c r="B335" t="inlineStr">
-        <is>
-          <t>Serious Infection</t>
-        </is>
-      </c>
-      <c r="C335">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="336">
-      <c r="A336">
-        <v>1075</v>
-      </c>
-      <c r="B336" t="inlineStr">
-        <is>
-          <t>Narcolepsy</t>
-        </is>
-      </c>
-      <c r="C336">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="337">
-      <c r="A337">
-        <v>1076</v>
-      </c>
-      <c r="B337" t="inlineStr">
-        <is>
-          <t>Anaphylaxis</t>
-        </is>
-      </c>
-      <c r="C337">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="338">
-      <c r="A338">
-        <v>1077</v>
-      </c>
-      <c r="B338" t="inlineStr">
-        <is>
-          <t>Anaphylaxis v2</t>
-        </is>
-      </c>
-      <c r="C338">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="339">
-      <c r="A339">
-        <v>1078</v>
-      </c>
-      <c r="B339" t="inlineStr">
-        <is>
-          <t>Bells Palsy</t>
-        </is>
-      </c>
-      <c r="C339">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="340">
-      <c r="A340">
-        <v>1079</v>
-      </c>
-      <c r="B340" t="inlineStr">
-        <is>
-          <t>Encephalomyelitis</t>
-        </is>
-      </c>
-      <c r="C340">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341">
-        <v>1080</v>
-      </c>
-      <c r="B341" t="inlineStr">
-        <is>
-          <t>Guillain Barre Syndrome</t>
-        </is>
-      </c>
-      <c r="C341">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="342">
-      <c r="A342">
-        <v>1081</v>
-      </c>
-      <c r="B342" t="inlineStr">
-        <is>
-          <t>Acute Myocardial Infarction including its complications</t>
-        </is>
-      </c>
-      <c r="C342">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="343">
-      <c r="A343">
-        <v>1082</v>
-      </c>
-      <c r="B343" t="inlineStr">
-        <is>
-          <t>Myocarditis Pericarditis</t>
-        </is>
-      </c>
-      <c r="C343">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="344">
-      <c r="A344">
-        <v>1083</v>
-      </c>
-      <c r="B344" t="inlineStr">
-        <is>
-          <t>Immune Thrombocytopenia (ITP)</t>
-        </is>
-      </c>
-      <c r="C344">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="345">
-      <c r="A345">
-        <v>1084</v>
-      </c>
-      <c r="B345" t="inlineStr">
-        <is>
-          <t>Disseminated Intravascular Coagulation</t>
-        </is>
-      </c>
-      <c r="C345">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="346">
-      <c r="A346">
-        <v>1085</v>
-      </c>
-      <c r="B346" t="inlineStr">
-        <is>
-          <t>Appendicitis</t>
-        </is>
-      </c>
-      <c r="C346">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="347">
-      <c r="A347">
-        <v>1086</v>
-      </c>
-      <c r="B347" t="inlineStr">
-        <is>
-          <t>Transverse Myelitis</t>
-        </is>
-      </c>
-      <c r="C347">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="348">
-      <c r="A348">
-        <v>1087</v>
-      </c>
-      <c r="B348" t="inlineStr">
-        <is>
-          <t>Hemorrhagic Stroke</t>
-        </is>
-      </c>
-      <c r="C348">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="349">
-      <c r="A349">
-        <v>1088</v>
-      </c>
-      <c r="B349" t="inlineStr">
-        <is>
-          <t>Deep Vein Thrombosis (DVT)</t>
-        </is>
-      </c>
-      <c r="C349">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="350">
-      <c r="A350">
-        <v>1089</v>
-      </c>
-      <c r="B350" t="inlineStr">
-        <is>
-          <t>Non-hemorrhagic Stroke</t>
-        </is>
-      </c>
-      <c r="C350">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="351">
-      <c r="A351">
-        <v>1090</v>
-      </c>
-      <c r="B351" t="inlineStr">
-        <is>
-          <t>Pulmonary Embolism</t>
-        </is>
-      </c>
-      <c r="C351">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="352">
-      <c r="A352">
-        <v>1091</v>
-      </c>
-      <c r="B352" t="inlineStr">
-        <is>
-          <t>Thrombosis with Thrombocytopenia (TWT)</t>
-        </is>
-      </c>
-      <c r="C352">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353">
-        <v>1093</v>
-      </c>
-      <c r="B353" t="inlineStr">
-        <is>
-          <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C353">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="354">
-      <c r="A354">
-        <v>1094</v>
-      </c>
-      <c r="B354" t="inlineStr">
-        <is>
-          <t>Lower Extremity Bypass - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C354">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="355">
-      <c r="A355">
-        <v>1095</v>
-      </c>
-      <c r="B355" t="inlineStr">
-        <is>
-          <t>Carotid Endarterectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C355">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="356">
-      <c r="A356">
-        <v>1096</v>
-      </c>
-      <c r="B356" t="inlineStr">
-        <is>
-          <t>Lung Resection - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C356">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="357">
-      <c r="A357">
-        <v>1097</v>
-      </c>
-      <c r="B357" t="inlineStr">
-        <is>
-          <t>Esophagectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C357">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="358">
-      <c r="A358">
-        <v>1098</v>
-      </c>
-      <c r="B358" t="inlineStr">
-        <is>
-          <t>Pancreatectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C358">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="359">
-      <c r="A359">
-        <v>1099</v>
-      </c>
-      <c r="B359" t="inlineStr">
-        <is>
-          <t>Colectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C359">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="360">
-      <c r="A360">
-        <v>1100</v>
-      </c>
-      <c r="B360" t="inlineStr">
-        <is>
-          <t>Cystectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C360">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="361">
-      <c r="A361">
-        <v>1101</v>
-      </c>
-      <c r="B361" t="inlineStr">
-        <is>
-          <t>Nephrectomy - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C361">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="362">
-      <c r="A362">
-        <v>1102</v>
-      </c>
-      <c r="B362" t="inlineStr">
-        <is>
-          <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C362">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="363">
-      <c r="A363">
-        <v>1103</v>
-      </c>
-      <c r="B363" t="inlineStr">
-        <is>
-          <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
-        </is>
-      </c>
-      <c r="C363">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="364">
-      <c r="A364">
-        <v>1104</v>
-      </c>
-      <c r="B364" t="inlineStr">
-        <is>
-          <t>RBC Transfusion (adult relevant, no auto 1yr clean window)</t>
-        </is>
-      </c>
-      <c r="C364">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="365">
-      <c r="A365">
-        <v>1105</v>
-      </c>
-      <c r="B365" t="inlineStr">
-        <is>
-          <t>Clostridium difficile - first episode</t>
-        </is>
-      </c>
-      <c r="C365">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="366">
-      <c r="A366">
-        <v>1106</v>
-      </c>
-      <c r="B366" t="inlineStr">
-        <is>
-          <t>Non-Emergent Major Non Cardiac Surgery no prior Opioid</t>
-        </is>
-      </c>
-      <c r="C366">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to how often specificaitons
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis1.xlsx
+++ b/analysis_specifications/analysis1.xlsx
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C263"/>
+  <dimension ref="A1:C262"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -420,7 +420,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
@@ -485,7 +485,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="8">
@@ -628,7 +628,7 @@
         </is>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="27">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="33">
@@ -901,7 +901,7 @@
         </is>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40">
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="48">
@@ -1031,7 +1031,7 @@
         </is>
       </c>
       <c r="C49">
-        <v>9999</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50">
@@ -1070,7 +1070,7 @@
         </is>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>365</v>
       </c>
     </row>
     <row r="53">
@@ -1096,7 +1096,7 @@
         </is>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="55">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="C92">
-        <v>365</v>
+        <v>180</v>
       </c>
     </row>
     <row r="93">
@@ -3168,11 +3168,11 @@
     </row>
     <row r="214">
       <c r="A214">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Earliest event of Neonatal Thrombocytopenia (NT), less than 1 year old</t>
+          <t>Earliest event of Warm Autoimmune Hemolytic Anemia (wAIHA)</t>
         </is>
       </c>
       <c r="C214">
@@ -3181,11 +3181,11 @@
     </row>
     <row r="215">
       <c r="A215">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Earliest event of Warm Autoimmune Hemolytic Anemia (wAIHA)</t>
+          <t>Earliest event of Major depressive disorder, with NO occurrence of certain psychiatric disorder</t>
         </is>
       </c>
       <c r="C215">
@@ -3194,11 +3194,11 @@
     </row>
     <row r="216">
       <c r="A216">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Earliest event of Major depressive disorder, with NO occurrence of certain psychiatric disorder</t>
+          <t>Earliest event of Myasthenia Gravis, inpatient, 2nd diagnosis or treatment, age gte 18</t>
         </is>
       </c>
       <c r="C216">
@@ -3207,11 +3207,11 @@
     </row>
     <row r="217">
       <c r="A217">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Earliest event of Myasthenia Gravis, inpatient, 2nd diagnosis or treatment, age gte 18</t>
+          <t>Earliest event of Depressive and Sleep Disorder</t>
         </is>
       </c>
       <c r="C217">
@@ -3220,11 +3220,11 @@
     </row>
     <row r="218">
       <c r="A218">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Earliest event of Depressive and Sleep Disorder</t>
+          <t>Earliest Event of Depressive Disorder with Suicidal Ideation or Attempt Prevalent</t>
         </is>
       </c>
       <c r="C218">
@@ -3233,11 +3233,11 @@
     </row>
     <row r="219">
       <c r="A219">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Earliest Event of Depressive Disorder with Suicidal Ideation or Attempt Prevalent</t>
+          <t>Earliest Event of Depressive Disorder with Anhedonia</t>
         </is>
       </c>
       <c r="C219">
@@ -3246,11 +3246,11 @@
     </row>
     <row r="220">
       <c r="A220">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Earliest Event of Depressive Disorder with Anhedonia</t>
+          <t>First event of Attention-deficit hyperactivity (ADHD) disorder or procedure</t>
         </is>
       </c>
       <c r="C220">
@@ -3259,11 +3259,11 @@
     </row>
     <row r="221">
       <c r="A221">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>First event of Attention-deficit hyperactivity (ADHD) disorder or procedure</t>
+          <t>Earliest Event of Multiple Sclerosis</t>
         </is>
       </c>
       <c r="C221">
@@ -3272,11 +3272,11 @@
     </row>
     <row r="222">
       <c r="A222">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Earliest Event of Multiple Sclerosis</t>
+          <t>Earliest event of Chronic Leukocytic Leukemia</t>
         </is>
       </c>
       <c r="C222">
@@ -3285,11 +3285,11 @@
     </row>
     <row r="223">
       <c r="A223">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Earliest event of Chronic Leukocytic Leukemia</t>
+          <t>Earliest event of Urothelial carcinoma</t>
         </is>
       </c>
       <c r="C223">
@@ -3298,11 +3298,11 @@
     </row>
     <row r="224">
       <c r="A224">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Earliest event of Urothelial carcinoma</t>
+          <t>Earliest event of Mantle Cell Lymphoma</t>
         </is>
       </c>
       <c r="C224">
@@ -3311,11 +3311,11 @@
     </row>
     <row r="225">
       <c r="A225">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Earliest event of Mantle Cell Lymphoma</t>
+          <t>Earliest event of Prostate cancer, among adult males</t>
         </is>
       </c>
       <c r="C225">
@@ -3324,11 +3324,11 @@
     </row>
     <row r="226">
       <c r="A226">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Earliest event of Prostate cancer, among adult males</t>
+          <t>Earliest event of Coronary artery disease (CAD)</t>
         </is>
       </c>
       <c r="C226">
@@ -3337,11 +3337,11 @@
     </row>
     <row r="227">
       <c r="A227">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Earliest event of Coronary artery disease (CAD)</t>
+          <t>Earliest event of Type 2 Diabetes Mellitus (DM), with no type 1 or secondary DM</t>
         </is>
       </c>
       <c r="C227">
@@ -3350,11 +3350,11 @@
     </row>
     <row r="228">
       <c r="A228">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Earliest event of Type 2 Diabetes Mellitus (DM), with no type 1 or secondary DM</t>
+          <t>Earliest event of Human Immunodeficiency Virus I (HIV), with treatment, lab or 2nd diagnosis</t>
         </is>
       </c>
       <c r="C228">
@@ -3363,50 +3363,50 @@
     </row>
     <row r="229">
       <c r="A229">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Earliest event of Human Immunodeficiency Virus I (HIV), with treatment, lab or 2nd diagnosis</t>
+          <t>All events of Respiratory syncytial virus infection, with 30 days washout</t>
         </is>
       </c>
       <c r="C229">
-        <v>9999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230">
       <c r="A230">
-        <v>1034</v>
+        <v>1072</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>All events of Respiratory syncytial virus infection, with 30 days washout</t>
+          <t>Cytomegalovirus CMV Anterior Uveitis</t>
         </is>
       </c>
       <c r="C230">
-        <v>0</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="231">
       <c r="A231">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Cytomegalovirus CMV Anterior Uveitis</t>
+          <t>Serious Infection, opportunistic infections and other infections of interest event</t>
         </is>
       </c>
       <c r="C231">
-        <v>9999</v>
+        <v>90</v>
       </c>
     </row>
     <row r="232">
       <c r="A232">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Serious Infection, opportunistic infections and other infections of interest event</t>
+          <t>Serious Infection</t>
         </is>
       </c>
       <c r="C232">
@@ -3415,50 +3415,50 @@
     </row>
     <row r="233">
       <c r="A233">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Serious Infection</t>
+          <t>Narcolepsy</t>
         </is>
       </c>
       <c r="C233">
-        <v>90</v>
+        <v>365</v>
       </c>
     </row>
     <row r="234">
       <c r="A234">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Narcolepsy</t>
+          <t>Anaphylaxis</t>
         </is>
       </c>
       <c r="C234">
-        <v>365</v>
+        <v>30</v>
       </c>
     </row>
     <row r="235">
       <c r="A235">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Anaphylaxis</t>
+          <t>Bells Palsy</t>
         </is>
       </c>
       <c r="C235">
-        <v>30</v>
+        <v>183</v>
       </c>
     </row>
     <row r="236">
       <c r="A236">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Bells Palsy</t>
+          <t>Encephalomyelitis</t>
         </is>
       </c>
       <c r="C236">
@@ -3467,24 +3467,24 @@
     </row>
     <row r="237">
       <c r="A237">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Encephalomyelitis</t>
+          <t>Guillain Barre Syndrome</t>
         </is>
       </c>
       <c r="C237">
-        <v>183</v>
+        <v>365</v>
       </c>
     </row>
     <row r="238">
       <c r="A238">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Guillain Barre Syndrome</t>
+          <t>Acute Myocardial Infarction including its complications</t>
         </is>
       </c>
       <c r="C238">
@@ -3493,11 +3493,11 @@
     </row>
     <row r="239">
       <c r="A239">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Acute Myocardial Infarction including its complications</t>
+          <t>Myocarditis Pericarditis</t>
         </is>
       </c>
       <c r="C239">
@@ -3506,11 +3506,11 @@
     </row>
     <row r="240">
       <c r="A240">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Myocarditis Pericarditis</t>
+          <t>Immune Thrombocytopenia (ITP)</t>
         </is>
       </c>
       <c r="C240">
@@ -3519,11 +3519,11 @@
     </row>
     <row r="241">
       <c r="A241">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Immune Thrombocytopenia (ITP)</t>
+          <t>Disseminated Intravascular Coagulation</t>
         </is>
       </c>
       <c r="C241">
@@ -3532,11 +3532,11 @@
     </row>
     <row r="242">
       <c r="A242">
-        <v>1084</v>
+        <v>1087</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Disseminated Intravascular Coagulation</t>
+          <t>Hemorrhagic Stroke</t>
         </is>
       </c>
       <c r="C242">
@@ -3545,11 +3545,11 @@
     </row>
     <row r="243">
       <c r="A243">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Hemorrhagic Stroke</t>
+          <t>Deep Vein Thrombosis (DVT)</t>
         </is>
       </c>
       <c r="C243">
@@ -3558,11 +3558,11 @@
     </row>
     <row r="244">
       <c r="A244">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Deep Vein Thrombosis (DVT)</t>
+          <t>Non-hemorrhagic Stroke</t>
         </is>
       </c>
       <c r="C244">
@@ -3571,11 +3571,11 @@
     </row>
     <row r="245">
       <c r="A245">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Non-hemorrhagic Stroke</t>
+          <t>Pulmonary Embolism</t>
         </is>
       </c>
       <c r="C245">
@@ -3584,11 +3584,11 @@
     </row>
     <row r="246">
       <c r="A246">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Pulmonary Embolism</t>
+          <t>Thrombosis with Thrombocytopenia (TWT)</t>
         </is>
       </c>
       <c r="C246">
@@ -3597,24 +3597,24 @@
     </row>
     <row r="247">
       <c r="A247">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Thrombosis with Thrombocytopenia (TWT)</t>
+          <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C247">
-        <v>365</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="248">
       <c r="A248">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
+          <t>Lower Extremity Bypass - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C248">
@@ -3623,11 +3623,11 @@
     </row>
     <row r="249">
       <c r="A249">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Lower Extremity Bypass - post op new Afib (any)</t>
+          <t>Carotid Endarterectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C249">
@@ -3636,11 +3636,11 @@
     </row>
     <row r="250">
       <c r="A250">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Carotid Endarterectomy - post op new Afib (any)</t>
+          <t>Lung Resection - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C250">
@@ -3649,11 +3649,11 @@
     </row>
     <row r="251">
       <c r="A251">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Lung Resection - post op new Afib (any)</t>
+          <t>Esophagectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C251">
@@ -3662,11 +3662,11 @@
     </row>
     <row r="252">
       <c r="A252">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Esophagectomy - post op new Afib (any)</t>
+          <t>Pancreatectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C252">
@@ -3675,11 +3675,11 @@
     </row>
     <row r="253">
       <c r="A253">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Pancreatectomy - post op new Afib (any)</t>
+          <t>Colectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C253">
@@ -3688,11 +3688,11 @@
     </row>
     <row r="254">
       <c r="A254">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Colectomy - post op new Afib (any)</t>
+          <t>Cystectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C254">
@@ -3701,11 +3701,11 @@
     </row>
     <row r="255">
       <c r="A255">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Cystectomy - post op new Afib (any)</t>
+          <t>Nephrectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C255">
@@ -3714,11 +3714,11 @@
     </row>
     <row r="256">
       <c r="A256">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Nephrectomy - post op new Afib (any)</t>
+          <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C256">
@@ -3727,11 +3727,11 @@
     </row>
     <row r="257">
       <c r="A257">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
+          <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C257">
@@ -3740,11 +3740,11 @@
     </row>
     <row r="258">
       <c r="A258">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
+          <t>RBC Transfusion (adult relevant, no auto 1yr clean window)</t>
         </is>
       </c>
       <c r="C258">
@@ -3753,11 +3753,11 @@
     </row>
     <row r="259">
       <c r="A259">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>RBC Transfusion (adult relevant, no auto 1yr clean window)</t>
+          <t>Clostridium difficile - first episode</t>
         </is>
       </c>
       <c r="C259">
@@ -3766,11 +3766,11 @@
     </row>
     <row r="260">
       <c r="A260">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Clostridium difficile - first episode</t>
+          <t>Non-Emergent Major Non Cardiac Surgery no prior Opioid</t>
         </is>
       </c>
       <c r="C260">
@@ -3779,11 +3779,11 @@
     </row>
     <row r="261">
       <c r="A261">
-        <v>1106</v>
+        <v>1150</v>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Non-Emergent Major Non Cardiac Surgery no prior Opioid</t>
+          <t>Emergency room visits (0Pe, 0Era)</t>
         </is>
       </c>
       <c r="C261">
@@ -3792,27 +3792,14 @@
     </row>
     <row r="262">
       <c r="A262">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>Emergency room visits (0Pe, 0Era)</t>
+          <t>Autism</t>
         </is>
       </c>
       <c r="C262">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263">
-        <v>1151</v>
-      </c>
-      <c r="B263" t="inlineStr">
-        <is>
-          <t>Autism</t>
-        </is>
-      </c>
-      <c r="C263">
         <v>9999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update to analysis 2 based on error report from evan
other small fixes
</commit_message>
<xml_diff>
--- a/analysis_specifications/analysis1.xlsx
+++ b/analysis_specifications/analysis1.xlsx
@@ -387,7 +387,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C266"/>
+  <dimension ref="A1:C265"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1127,11 +1127,11 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Inflammatory Bowel Disease</t>
+          <t>Pulmonary Arterial Hypertension</t>
         </is>
       </c>
       <c r="C57">
@@ -1140,11 +1140,11 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Pulmonary Arterial Hypertension</t>
+          <t>Psoriatic arthritis</t>
         </is>
       </c>
       <c r="C58">
@@ -1153,11 +1153,11 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Psoriatic arthritis</t>
+          <t>Plaque Psoriasis</t>
         </is>
       </c>
       <c r="C59">
@@ -1166,11 +1166,11 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Plaque Psoriasis</t>
+          <t>Pulmonary hypertension associated with left heart disease (WHO Group 2)</t>
         </is>
       </c>
       <c r="C60">
@@ -1179,11 +1179,11 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Pulmonary hypertension associated with left heart disease (WHO Group 2)</t>
+          <t>Pulmonary hypertension associated with lung diseases and/or hypoxia (WHO Group 3)</t>
         </is>
       </c>
       <c r="C61">
@@ -1192,11 +1192,11 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Pulmonary hypertension associated with lung diseases and/or hypoxia (WHO Group 3)</t>
+          <t>Firearm Accidents (FA)</t>
         </is>
       </c>
       <c r="C62">
@@ -1205,37 +1205,37 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Firearm Accidents (FA)</t>
+          <t>Motor Vehicle Accidents (MVA)</t>
         </is>
       </c>
       <c r="C63">
-        <v>9999</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64">
       <c r="A64">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Motor Vehicle Accidents (MVA)</t>
+          <t>Down Syndrome</t>
         </is>
       </c>
       <c r="C64">
-        <v>180</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="65">
       <c r="A65">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Down Syndrome</t>
+          <t>Non-infectious uveitis and iridocyclitis</t>
         </is>
       </c>
       <c r="C65">
@@ -1244,11 +1244,11 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Non-infectious uveitis and iridocyclitis</t>
+          <t>Cystic Fibrosis</t>
         </is>
       </c>
       <c r="C66">
@@ -1257,11 +1257,11 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Cystic Fibrosis</t>
+          <t>Concomitant TNF - alpha Inhibitors and IL12_23 Inhibitors - GE 30D overlap</t>
         </is>
       </c>
       <c r="C67">
@@ -1270,11 +1270,11 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Concomitant TNF - alpha Inhibitors and IL12_23 Inhibitors - GE 30D overlap</t>
+          <t>Concomitant TNF - alpha Inhibitors and IL23 Inhibitors - GE 30D overlap</t>
         </is>
       </c>
       <c r="C68">
@@ -1283,11 +1283,11 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Concomitant TNF - alpha Inhibitors and IL23 Inhibitors - GE 30D overlap</t>
+          <t>Concomitant IL 23 Inhibitors and IL12_23 Inhibitors - GE 30D overlap</t>
         </is>
       </c>
       <c r="C69">
@@ -1296,11 +1296,11 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Concomitant IL 23 Inhibitors and IL12_23 Inhibitors - GE 30D overlap</t>
+          <t>Pulmonary arterial hypertension with Prior Left Heart or Vice Versa</t>
         </is>
       </c>
       <c r="C70">
@@ -1309,11 +1309,11 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Pulmonary arterial hypertension with Prior Left Heart or Vice Versa</t>
+          <t>Endothelin receptor antagonists</t>
         </is>
       </c>
       <c r="C71">
@@ -1322,11 +1322,11 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Endothelin receptor antagonists</t>
+          <t>Phosphodiesterase 5 inhibitors and guanylate cyclase stimulators</t>
         </is>
       </c>
       <c r="C72">
@@ -1335,11 +1335,11 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Phosphodiesterase 5 inhibitors and guanylate cyclase stimulators</t>
+          <t>Prostacyclin analogues and prostacyclin receptor agonists</t>
         </is>
       </c>
       <c r="C73">
@@ -1348,11 +1348,11 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Prostacyclin analogues and prostacyclin receptor agonists</t>
+          <t>Left Heart Failure</t>
         </is>
       </c>
       <c r="C74">
@@ -1361,11 +1361,11 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Left Heart Failure</t>
+          <t>Right Heart Failure</t>
         </is>
       </c>
       <c r="C75">
@@ -1374,11 +1374,11 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Right Heart Failure</t>
+          <t>Sarcoidosis</t>
         </is>
       </c>
       <c r="C76">
@@ -1387,11 +1387,11 @@
     </row>
     <row r="77">
       <c r="A77">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Sarcoidosis</t>
+          <t>Sickle Cell Anemia</t>
         </is>
       </c>
       <c r="C77">
@@ -1400,11 +1400,11 @@
     </row>
     <row r="78">
       <c r="A78">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Sickle Cell Anemia</t>
+          <t>Scleroderma</t>
         </is>
       </c>
       <c r="C78">
@@ -1413,11 +1413,11 @@
     </row>
     <row r="79">
       <c r="A79">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Scleroderma</t>
+          <t>Essential Hypertension</t>
         </is>
       </c>
       <c r="C79">
@@ -1426,11 +1426,11 @@
     </row>
     <row r="80">
       <c r="A80">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Essential Hypertension</t>
+          <t>Congenital Heart Disease</t>
         </is>
       </c>
       <c r="C80">
@@ -1439,11 +1439,11 @@
     </row>
     <row r="81">
       <c r="A81">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Congenital Heart Disease</t>
+          <t>Portal Hypertension</t>
         </is>
       </c>
       <c r="C81">
@@ -1452,11 +1452,11 @@
     </row>
     <row r="82">
       <c r="A82">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Portal Hypertension</t>
+          <t>Inflammatory Bowel Disease</t>
         </is>
       </c>
       <c r="C82">
@@ -1465,11 +1465,11 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Inflammatory Bowel Disease</t>
+          <t>Antisynthetase syndrome</t>
         </is>
       </c>
       <c r="C83">
@@ -1478,11 +1478,11 @@
     </row>
     <row r="84">
       <c r="A84">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Antisynthetase syndrome</t>
+          <t>Mixed connective tissue disease</t>
         </is>
       </c>
       <c r="C84">
@@ -1491,11 +1491,11 @@
     </row>
     <row r="85">
       <c r="A85">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Mixed connective tissue disease</t>
+          <t>Undifferentiated connective tissue disease</t>
         </is>
       </c>
       <c r="C85">
@@ -1504,11 +1504,11 @@
     </row>
     <row r="86">
       <c r="A86">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Undifferentiated connective tissue disease</t>
+          <t>Overlap syndrome</t>
         </is>
       </c>
       <c r="C86">
@@ -1517,11 +1517,11 @@
     </row>
     <row r="87">
       <c r="A87">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Overlap syndrome</t>
+          <t>Raynaud’s disease or Raynaud’s phenomenon</t>
         </is>
       </c>
       <c r="C87">
@@ -1530,11 +1530,11 @@
     </row>
     <row r="88">
       <c r="A88">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Raynaud’s disease or Raynaud’s phenomenon</t>
+          <t>Antiphospholipid syndrome</t>
         </is>
       </c>
       <c r="C88">
@@ -1543,11 +1543,11 @@
     </row>
     <row r="89">
       <c r="A89">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Antiphospholipid syndrome</t>
+          <t>Chronic Thromboembolic Pulmonary Hypertension</t>
         </is>
       </c>
       <c r="C89">
@@ -1556,24 +1556,24 @@
     </row>
     <row r="90">
       <c r="A90">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Chronic Thromboembolic Pulmonary Hypertension</t>
+          <t>Pulmonary endarterectomy</t>
         </is>
       </c>
       <c r="C90">
-        <v>9999</v>
+        <v>30</v>
       </c>
     </row>
     <row r="91">
       <c r="A91">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Pulmonary endarterectomy</t>
+          <t>Balloon Pulmonary Angioplasty</t>
         </is>
       </c>
       <c r="C91">
@@ -1582,37 +1582,37 @@
     </row>
     <row r="92">
       <c r="A92">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Balloon Pulmonary Angioplasty</t>
+          <t>Skin Burns</t>
         </is>
       </c>
       <c r="C92">
-        <v>30</v>
+        <v>180</v>
       </c>
     </row>
     <row r="93">
       <c r="A93">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Skin Burns</t>
+          <t>Non-small cell lung cancer (NSCLC)</t>
         </is>
       </c>
       <c r="C93">
-        <v>180</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="94">
       <c r="A94">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Non-small cell lung cancer (NSCLC)</t>
+          <t>Lung cancer</t>
         </is>
       </c>
       <c r="C94">
@@ -1621,11 +1621,11 @@
     </row>
     <row r="95">
       <c r="A95">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Lung cancer</t>
+          <t>Breast cancer</t>
         </is>
       </c>
       <c r="C95">
@@ -1634,11 +1634,11 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Breast cancer</t>
+          <t>Glioblastoma multiforme (GBM)</t>
         </is>
       </c>
       <c r="C96">
@@ -1647,11 +1647,11 @@
     </row>
     <row r="97">
       <c r="A97">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Glioblastoma multiforme (GBM)</t>
+          <t>Colorectal Cancer</t>
         </is>
       </c>
       <c r="C97">
@@ -1660,11 +1660,11 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Colorectal Cancer</t>
+          <t>Multiple Myeloma</t>
         </is>
       </c>
       <c r="C98">
@@ -1673,11 +1673,11 @@
     </row>
     <row r="99">
       <c r="A99">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Multiple Myeloma</t>
+          <t>Metastatic Hormone-Sensitive Prostate Cancer Synchronous</t>
         </is>
       </c>
       <c r="C99">
@@ -1686,11 +1686,11 @@
     </row>
     <row r="100">
       <c r="A100">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Metastatic Hormone-Sensitive Prostate Cancer Synchronous</t>
+          <t>Metastatic Hormone-Sensitive Prostate Cancer Metachronus</t>
         </is>
       </c>
       <c r="C100">
@@ -1699,11 +1699,11 @@
     </row>
     <row r="101">
       <c r="A101">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Metastatic Hormone-Sensitive Prostate Cancer Metachronus</t>
+          <t>Antineoplastic drugs against colorectal cancer</t>
         </is>
       </c>
       <c r="C101">
@@ -1712,11 +1712,11 @@
     </row>
     <row r="102">
       <c r="A102">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Antineoplastic drugs against colorectal cancer</t>
+          <t>Potential curative surgery for colorectal cancer</t>
         </is>
       </c>
       <c r="C102">
@@ -1725,11 +1725,11 @@
     </row>
     <row r="103">
       <c r="A103">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Potential curative surgery for colorectal cancer</t>
+          <t>Radiotherapy against colorectal cancer</t>
         </is>
       </c>
       <c r="C103">
@@ -1738,11 +1738,11 @@
     </row>
     <row r="104">
       <c r="A104">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>Radiotherapy against colorectal cancer</t>
+          <t>Primary adenocarcinoma of the colon or rectum</t>
         </is>
       </c>
       <c r="C104">
@@ -1751,11 +1751,11 @@
     </row>
     <row r="105">
       <c r="A105">
-        <v>798</v>
+        <v>802</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum</t>
+          <t>Acute Respiratory Failure</t>
         </is>
       </c>
       <c r="C105">
@@ -1764,11 +1764,11 @@
     </row>
     <row r="106">
       <c r="A106">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Acute Respiratory Failure</t>
+          <t>Fascial dehiscence and evisceration</t>
         </is>
       </c>
       <c r="C106">
@@ -1777,11 +1777,11 @@
     </row>
     <row r="107">
       <c r="A107">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Fascial dehiscence and evisceration</t>
+          <t>Anastomotic leak or dehiscence</t>
         </is>
       </c>
       <c r="C107">
@@ -1790,11 +1790,11 @@
     </row>
     <row r="108">
       <c r="A108">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Anastomotic leak or dehiscence</t>
+          <t>Intestinal obstruction</t>
         </is>
       </c>
       <c r="C108">
@@ -1803,11 +1803,11 @@
     </row>
     <row r="109">
       <c r="A109">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Intestinal obstruction</t>
+          <t>Intraabdominal abscess</t>
         </is>
       </c>
       <c r="C109">
@@ -1816,11 +1816,11 @@
     </row>
     <row r="110">
       <c r="A110">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Intraabdominal abscess</t>
+          <t>Perioperative aspiration</t>
         </is>
       </c>
       <c r="C110">
@@ -1829,11 +1829,11 @@
     </row>
     <row r="111">
       <c r="A111">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Perioperative aspiration</t>
+          <t>Postoperative hemorrhage</t>
         </is>
       </c>
       <c r="C111">
@@ -1842,11 +1842,11 @@
     </row>
     <row r="112">
       <c r="A112">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Postoperative hemorrhage</t>
+          <t>Surgical wound infection (narrow)</t>
         </is>
       </c>
       <c r="C112">
@@ -1855,11 +1855,11 @@
     </row>
     <row r="113">
       <c r="A113">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Surgical wound infection (narrow)</t>
+          <t>Distant metastasis following colorectal cancer (wide)</t>
         </is>
       </c>
       <c r="C113">
@@ -1868,11 +1868,11 @@
     </row>
     <row r="114">
       <c r="A114">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Distant metastasis following colorectal cancer (wide)</t>
+          <t>Local recurrence after colorectal cancer</t>
         </is>
       </c>
       <c r="C114">
@@ -1881,11 +1881,11 @@
     </row>
     <row r="115">
       <c r="A115">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Local recurrence after colorectal cancer</t>
+          <t>Primary adenocarcinoma of the colon or rectum, MSI-H or dMMR, no surgery or oncological treatment</t>
         </is>
       </c>
       <c r="C115">
@@ -1894,11 +1894,11 @@
     </row>
     <row r="116">
       <c r="A116">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum, MSI-H or dMMR, no surgery or oncological treatment</t>
+          <t>Primary adenocarcinoma of the colon or rectum treated with potentially curative surgery</t>
         </is>
       </c>
       <c r="C116">
@@ -1907,11 +1907,11 @@
     </row>
     <row r="117">
       <c r="A117">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum treated with potentially curative surgery</t>
+          <t>Primary adenocarcinoma of the colon or rectum, no curative intended surgery and oncological treatment</t>
         </is>
       </c>
       <c r="C117">
@@ -1920,7 +1920,7 @@
     </row>
     <row r="118">
       <c r="A118">
-        <v>814</v>
+        <v>817</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -1933,11 +1933,11 @@
     </row>
     <row r="119">
       <c r="A119">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum, no curative intended surgery and oncological treatment</t>
+          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR</t>
         </is>
       </c>
       <c r="C119">
@@ -1946,11 +1946,11 @@
     </row>
     <row r="120">
       <c r="A120">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR</t>
+          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR, treated with curative intended surgery</t>
         </is>
       </c>
       <c r="C120">
@@ -1959,11 +1959,11 @@
     </row>
     <row r="121">
       <c r="A121">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR, treated with curative intended surgery</t>
+          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR, oncological treatment, no curative surgery</t>
         </is>
       </c>
       <c r="C121">
@@ -1972,11 +1972,11 @@
     </row>
     <row r="122">
       <c r="A122">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR, oncological treatment, no curative surgery</t>
+          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR, no surgery or oncological treatment</t>
         </is>
       </c>
       <c r="C122">
@@ -1985,11 +1985,11 @@
     </row>
     <row r="123">
       <c r="A123">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of the colon or rectum, MSI-L, MSI-indeterminate, MSS or pMMR, no surgery or oncological treatment</t>
+          <t>Primary adenocarcinoma of colon or rectum, MSI-H or dMMR, surgical treatment</t>
         </is>
       </c>
       <c r="C123">
@@ -1998,11 +1998,11 @@
     </row>
     <row r="124">
       <c r="A124">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon or rectum, MSI-H or dMMR, surgical treatment</t>
+          <t>Primary adenocarcinoma of colon or rectum, MSI-H or dMMR, oncological treatment no surgery</t>
         </is>
       </c>
       <c r="C124">
@@ -2011,11 +2011,11 @@
     </row>
     <row r="125">
       <c r="A125">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon or rectum, MSI-H or dMMR, oncological treatment no surgery</t>
+          <t>Primary adenocarcinoma of colon or rectum, MSI-H or dMMR</t>
         </is>
       </c>
       <c r="C125">
@@ -2024,11 +2024,11 @@
     </row>
     <row r="126">
       <c r="A126">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon or rectum, MSI-H or dMMR</t>
+          <t>Primary adenocarcinoma of colon</t>
         </is>
       </c>
       <c r="C126">
@@ -2037,11 +2037,11 @@
     </row>
     <row r="127">
       <c r="A127">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon</t>
+          <t>Primary adenocarcinoma of colon, no surgery or oncological treatment</t>
         </is>
       </c>
       <c r="C127">
@@ -2050,11 +2050,11 @@
     </row>
     <row r="128">
       <c r="A128">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon, no surgery or oncological treatment</t>
+          <t>Primary adenocarcinoma of colon surgical treatment</t>
         </is>
       </c>
       <c r="C128">
@@ -2063,11 +2063,11 @@
     </row>
     <row r="129">
       <c r="A129">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon surgical treatment</t>
+          <t>Primary adenocarcinoma of colon oncological treatment, no surgery</t>
         </is>
       </c>
       <c r="C129">
@@ -2076,11 +2076,11 @@
     </row>
     <row r="130">
       <c r="A130">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon oncological treatment, no surgery</t>
+          <t>Primary adenocarcinoma of colon, MSI-L, MSI-indeterminate, MSS or pMMR</t>
         </is>
       </c>
       <c r="C130">
@@ -2089,11 +2089,11 @@
     </row>
     <row r="131">
       <c r="A131">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon, MSI-L, MSI-indeterminate, MSS or pMMR</t>
+          <t>Primary adenocarcinoma of colon, MSI-L, MSI-indeterminate, MSS or pMMR, surgically treated</t>
         </is>
       </c>
       <c r="C131">
@@ -2102,11 +2102,11 @@
     </row>
     <row r="132">
       <c r="A132">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon, MSI-L, MSI-indeterminate, MSS or pMMR, surgically treated</t>
+          <t>Primary adenocarcinoma of colon MSI-L, MSI-indeterminate, MSS or pMMR, oncological treatment, no surgery</t>
         </is>
       </c>
       <c r="C132">
@@ -2115,11 +2115,11 @@
     </row>
     <row r="133">
       <c r="A133">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon MSI-L, MSI-indeterminate, MSS or pMMR, oncological treatment, no surgery</t>
+          <t>Primary adenocarcinoma of colon MSI-L, MSI-indeterminate, MSS or pMMR, no surgery or oncological treatment</t>
         </is>
       </c>
       <c r="C133">
@@ -2128,11 +2128,11 @@
     </row>
     <row r="134">
       <c r="A134">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon MSI-L, MSI-indeterminate, MSS or pMMR, no surgery or oncological treatment</t>
+          <t>Primary adenocarcinoma of colon MSI-H or dMMR</t>
         </is>
       </c>
       <c r="C134">
@@ -2141,11 +2141,11 @@
     </row>
     <row r="135">
       <c r="A135">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon MSI-H or dMMR</t>
+          <t>Primary adenocarcinoma of colon MSI-H or dMMR, surgical treatment</t>
         </is>
       </c>
       <c r="C135">
@@ -2154,11 +2154,11 @@
     </row>
     <row r="136">
       <c r="A136">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon MSI-H or dMMR, surgical treatment</t>
+          <t>Primary adenocarcinoma of colon MSI-H or dMMR, oncological treatment, no surgery</t>
         </is>
       </c>
       <c r="C136">
@@ -2167,11 +2167,11 @@
     </row>
     <row r="137">
       <c r="A137">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon MSI-H or dMMR, oncological treatment, no surgery</t>
+          <t>Primary adenocarcinoma of colon MSI-H or dMMR, no surgery or oncological treatment</t>
         </is>
       </c>
       <c r="C137">
@@ -2180,11 +2180,11 @@
     </row>
     <row r="138">
       <c r="A138">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of colon MSI-H or dMMR, no surgery or oncological treatment</t>
+          <t>Primary adenocarcinoma of rectum</t>
         </is>
       </c>
       <c r="C138">
@@ -2193,11 +2193,11 @@
     </row>
     <row r="139">
       <c r="A139">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum</t>
+          <t>Primary adenocarcinoma of rectum MSI-H or dMMR</t>
         </is>
       </c>
       <c r="C139">
@@ -2206,11 +2206,11 @@
     </row>
     <row r="140">
       <c r="A140">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum MSI-H or dMMR</t>
+          <t>Primary adenocarcinoma of rectum, MSI-H or dMMR, no surgery or oncological treatment</t>
         </is>
       </c>
       <c r="C140">
@@ -2219,11 +2219,11 @@
     </row>
     <row r="141">
       <c r="A141">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum, MSI-H or dMMR, no surgery or oncological treatment</t>
+          <t>Primary adenocarcinoma of rectum MSI-H or dMMR, oncological treatment, no surgery</t>
         </is>
       </c>
       <c r="C141">
@@ -2232,11 +2232,11 @@
     </row>
     <row r="142">
       <c r="A142">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum MSI-H or dMMR, oncological treatment, no surgery</t>
+          <t>Primary adenocarcinoma of rectum, MSI-H or dMMR, surgical treatment</t>
         </is>
       </c>
       <c r="C142">
@@ -2245,11 +2245,11 @@
     </row>
     <row r="143">
       <c r="A143">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum, MSI-H or dMMR, surgical treatment</t>
+          <t>Primary adenocarcinoma of rectum, MSI-L, MSI-indeterminate, MSS or pMMR</t>
         </is>
       </c>
       <c r="C143">
@@ -2258,11 +2258,11 @@
     </row>
     <row r="144">
       <c r="A144">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum, MSI-L, MSI-indeterminate, MSS or pMMR</t>
+          <t>Primary adenocarcinoma of rectum MSI-L, MSI-indeterminate, MSS or pMMR, oncological treatment, no surgery</t>
         </is>
       </c>
       <c r="C144">
@@ -2271,11 +2271,11 @@
     </row>
     <row r="145">
       <c r="A145">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum MSI-L, MSI-indeterminate, MSS or pMMR, oncological treatment, no surgery</t>
+          <t>Primary adenocarcinoma of rectum MSI-L, MSI-indeterminate, MSS or pMMR, no surgery and no oncological treatment</t>
         </is>
       </c>
       <c r="C145">
@@ -2284,11 +2284,11 @@
     </row>
     <row r="146">
       <c r="A146">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum MSI-L, MSI-indeterminate, MSS or pMMR, no surgery and no oncological treatment</t>
+          <t>Primary adenocarcinoma of rectum MSI-L, MSI-indeterminate, MSS or pMMR, treated with potentially curative surgery</t>
         </is>
       </c>
       <c r="C146">
@@ -2297,11 +2297,11 @@
     </row>
     <row r="147">
       <c r="A147">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum MSI-L, MSI-indeterminate, MSS or pMMR, treated with potentially curative surgery</t>
+          <t>Primary adenocarcinoma of rectum oncological treatment, no surgery</t>
         </is>
       </c>
       <c r="C147">
@@ -2310,11 +2310,11 @@
     </row>
     <row r="148">
       <c r="A148">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum oncological treatment, no surgery</t>
+          <t>Primary adenocarcinoma of rectum surgical treatment</t>
         </is>
       </c>
       <c r="C148">
@@ -2323,11 +2323,11 @@
     </row>
     <row r="149">
       <c r="A149">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum surgical treatment</t>
+          <t>Primary adenocarcinoma of rectum, no surgery or oncological treatment</t>
         </is>
       </c>
       <c r="C149">
@@ -2336,11 +2336,11 @@
     </row>
     <row r="150">
       <c r="A150">
-        <v>848</v>
+        <v>851</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Primary adenocarcinoma of rectum, no surgery or oncological treatment</t>
+          <t>Intraabdominal obstruction</t>
         </is>
       </c>
       <c r="C150">
@@ -2349,11 +2349,11 @@
     </row>
     <row r="151">
       <c r="A151">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Intraabdominal obstruction</t>
+          <t>Surgical wound infection (broad)</t>
         </is>
       </c>
       <c r="C151">
@@ -2362,11 +2362,11 @@
     </row>
     <row r="152">
       <c r="A152">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Surgical wound infection (broad)</t>
+          <t>Distant metastasis following colorectal cancer (medium)</t>
         </is>
       </c>
       <c r="C152">
@@ -2375,11 +2375,11 @@
     </row>
     <row r="153">
       <c r="A153">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Distant metastasis following colorectal cancer (medium)</t>
+          <t>Distant metastasis following colorectal cancer (narrow)</t>
         </is>
       </c>
       <c r="C153">
@@ -2388,11 +2388,11 @@
     </row>
     <row r="154">
       <c r="A154">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Distant metastasis following colorectal cancer (narrow)</t>
+          <t>Earliest event of Migraine</t>
         </is>
       </c>
       <c r="C154">
@@ -2401,11 +2401,11 @@
     </row>
     <row r="155">
       <c r="A155">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Earliest event of Migraine</t>
+          <t>Earliest event of Rheumatoid Arthritis</t>
         </is>
       </c>
       <c r="C155">
@@ -2414,11 +2414,11 @@
     </row>
     <row r="156">
       <c r="A156">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Earliest event of Rheumatoid Arthritis</t>
+          <t>Earliest event of Crohns disease</t>
         </is>
       </c>
       <c r="C156">
@@ -2427,11 +2427,11 @@
     </row>
     <row r="157">
       <c r="A157">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Earliest event of Crohns disease</t>
+          <t>Earliest event of Ulcerative colitis</t>
         </is>
       </c>
       <c r="C157">
@@ -2440,11 +2440,11 @@
     </row>
     <row r="158">
       <c r="A158">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Earliest event of Ulcerative colitis</t>
+          <t>Earliest event of Urinary tract infections (UTI)</t>
         </is>
       </c>
       <c r="C158">
@@ -2453,11 +2453,11 @@
     </row>
     <row r="159">
       <c r="A159">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Earliest event of Urinary tract infections (UTI)</t>
+          <t>Earliest event of Alzheimer's disease derived from Imfeld, 2</t>
         </is>
       </c>
       <c r="C159">
@@ -2466,11 +2466,11 @@
     </row>
     <row r="160">
       <c r="A160">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Earliest event of Alzheimer's disease derived from Imfeld, 2</t>
+          <t>Cognitive impairment, incident</t>
         </is>
       </c>
       <c r="C160">
@@ -2479,11 +2479,11 @@
     </row>
     <row r="161">
       <c r="A161">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Cognitive impairment, incident</t>
+          <t>Earliest event of Dementia</t>
         </is>
       </c>
       <c r="C161">
@@ -2492,11 +2492,11 @@
     </row>
     <row r="162">
       <c r="A162">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Earliest event of Dementia</t>
+          <t>Non-Emergent Major Non Cardiac Surgery among adults</t>
         </is>
       </c>
       <c r="C162">
@@ -2505,11 +2505,11 @@
     </row>
     <row r="163">
       <c r="A163">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Non-Emergent Major Non Cardiac Surgery among adults</t>
+          <t>AAA repair among adults with new onset atrial fibrillation after surgery</t>
         </is>
       </c>
       <c r="C163">
@@ -2518,11 +2518,11 @@
     </row>
     <row r="164">
       <c r="A164">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>AAA repair among adults with new onset atrial fibrillation after surgery</t>
+          <t>Lower Extremity Bypass among adults</t>
         </is>
       </c>
       <c r="C164">
@@ -2531,11 +2531,11 @@
     </row>
     <row r="165">
       <c r="A165">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Lower Extremity Bypass among adults</t>
+          <t>Carotid Endarterectomy among adults</t>
         </is>
       </c>
       <c r="C165">
@@ -2544,11 +2544,11 @@
     </row>
     <row r="166">
       <c r="A166">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Carotid Endarterectomy among adults</t>
+          <t>Lung Resection among adults</t>
         </is>
       </c>
       <c r="C166">
@@ -2557,11 +2557,11 @@
     </row>
     <row r="167">
       <c r="A167">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Lung Resection among adults</t>
+          <t>Esophagectomy among adults</t>
         </is>
       </c>
       <c r="C167">
@@ -2570,11 +2570,11 @@
     </row>
     <row r="168">
       <c r="A168">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Esophagectomy among adults</t>
+          <t>Pancreatectomy among adults</t>
         </is>
       </c>
       <c r="C168">
@@ -2583,11 +2583,11 @@
     </row>
     <row r="169">
       <c r="A169">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Pancreatectomy among adults</t>
+          <t>Colectomy among adults</t>
         </is>
       </c>
       <c r="C169">
@@ -2596,11 +2596,11 @@
     </row>
     <row r="170">
       <c r="A170">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Colectomy among adults</t>
+          <t>Cystectomy among adults</t>
         </is>
       </c>
       <c r="C170">
@@ -2609,11 +2609,11 @@
     </row>
     <row r="171">
       <c r="A171">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Cystectomy among adults</t>
+          <t>Nephrectomy among adults</t>
         </is>
       </c>
       <c r="C171">
@@ -2622,11 +2622,11 @@
     </row>
     <row r="172">
       <c r="A172">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Nephrectomy among adults</t>
+          <t>Coronary Artery Bypass Graft Surgery among adults</t>
         </is>
       </c>
       <c r="C172">
@@ -2635,11 +2635,11 @@
     </row>
     <row r="173">
       <c r="A173">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Coronary Artery Bypass Graft Surgery among adults</t>
+          <t>Aortic or Mitral Valve Repair or Replacement among adults</t>
         </is>
       </c>
       <c r="C173">
@@ -2648,11 +2648,11 @@
     </row>
     <row r="174">
       <c r="A174">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Aortic or Mitral Valve Repair or Replacement among adults</t>
+          <t>Non-Emergent MNCS (age 18 or greater), post op Afib (parox)</t>
         </is>
       </c>
       <c r="C174">
@@ -2661,11 +2661,11 @@
     </row>
     <row r="175">
       <c r="A175">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Non-Emergent MNCS (age 18 or greater), post op Afib (parox)</t>
+          <t>Non-Emergent MNCS (age 18 or greater), post op Afib (any)</t>
         </is>
       </c>
       <c r="C175">
@@ -2674,24 +2674,24 @@
     </row>
     <row r="176">
       <c r="A176">
-        <v>878</v>
+        <v>884</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Non-Emergent MNCS (age 18 or greater), post op Afib (any)</t>
+          <t>Diarrhea events</t>
         </is>
       </c>
       <c r="C176">
-        <v>9999</v>
+        <v>30</v>
       </c>
     </row>
     <row r="177">
       <c r="A177">
-        <v>884</v>
+        <v>888</v>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Diarrhea events</t>
+          <t>Gastrointestinal bleeding events</t>
         </is>
       </c>
       <c r="C177">
@@ -2700,24 +2700,24 @@
     </row>
     <row r="178">
       <c r="A178">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Gastrointestinal bleeding events</t>
+          <t>Hyponatremia events</t>
         </is>
       </c>
       <c r="C178">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="179">
       <c r="A179">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Hyponatremia events</t>
+          <t>Hypotension events</t>
         </is>
       </c>
       <c r="C179">
@@ -2726,63 +2726,63 @@
     </row>
     <row r="180">
       <c r="A180">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Hypotension events</t>
+          <t>Nausea events</t>
         </is>
       </c>
       <c r="C180">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="181">
       <c r="A181">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Nausea events</t>
+          <t>Stroke (ischemic or hemorrhagic) events</t>
         </is>
       </c>
       <c r="C181">
-        <v>30</v>
+        <v>180</v>
       </c>
     </row>
     <row r="182">
       <c r="A182">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Stroke (ischemic or hemorrhagic) events</t>
+          <t>Persons with vertigo</t>
         </is>
       </c>
       <c r="C182">
-        <v>180</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="183">
       <c r="A183">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Persons with vertigo</t>
+          <t>Abdominal pain events</t>
         </is>
       </c>
       <c r="C183">
-        <v>9999</v>
+        <v>90</v>
       </c>
     </row>
     <row r="184">
       <c r="A184">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Abdominal pain events</t>
+          <t>Abnormal weight gain events</t>
         </is>
       </c>
       <c r="C184">
@@ -2791,11 +2791,11 @@
     </row>
     <row r="185">
       <c r="A185">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Abnormal weight gain events</t>
+          <t>Abnormal weight loss events</t>
         </is>
       </c>
       <c r="C185">
@@ -2804,37 +2804,37 @@
     </row>
     <row r="186">
       <c r="A186">
-        <v>896</v>
+        <v>920</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Abnormal weight loss events</t>
+          <t>Total cardiovascular disease events (ischemic stroke, hemorrhagic stroke, heart failure, acute myocardial infarction or sudden cardiac death)</t>
         </is>
       </c>
       <c r="C186">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="187">
       <c r="A187">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Total cardiovascular disease events (ischemic stroke, hemorrhagic stroke, heart failure, acute myocardial infarction or sudden cardiac death)</t>
+          <t>Cardiovascular-related mortality</t>
         </is>
       </c>
       <c r="C187">
-        <v>180</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Cardiovascular-related mortality</t>
+          <t>Persons with chronic kidney disease</t>
         </is>
       </c>
       <c r="C188">
@@ -2843,102 +2843,102 @@
     </row>
     <row r="189">
       <c r="A189">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Persons with chronic kidney disease</t>
+          <t>Cough events</t>
         </is>
       </c>
       <c r="C189">
-        <v>9999</v>
+        <v>90</v>
       </c>
     </row>
     <row r="190">
       <c r="A190">
-        <v>925</v>
+        <v>929</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Cough events</t>
+          <t>Edema events</t>
         </is>
       </c>
       <c r="C190">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Edema events</t>
+          <t>Persons with end stage renal disease</t>
         </is>
       </c>
       <c r="C191">
-        <v>180</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="192">
       <c r="A192">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Persons with end stage renal disease</t>
+          <t>Fall events</t>
         </is>
       </c>
       <c r="C192">
-        <v>9999</v>
+        <v>180</v>
       </c>
     </row>
     <row r="193">
       <c r="A193">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Fall events</t>
+          <t>Persons with gout</t>
         </is>
       </c>
       <c r="C193">
-        <v>180</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="194">
       <c r="A194">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Persons with gout</t>
+          <t>Headache events</t>
         </is>
       </c>
       <c r="C194">
-        <v>9999</v>
+        <v>30</v>
       </c>
     </row>
     <row r="195">
       <c r="A195">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Headache events</t>
+          <t>Persons with heart failure</t>
         </is>
       </c>
       <c r="C195">
-        <v>30</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>934</v>
+        <v>936</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Persons with heart failure</t>
+          <t>Persons with hepatic failure</t>
         </is>
       </c>
       <c r="C196">
@@ -2947,37 +2947,37 @@
     </row>
     <row r="197">
       <c r="A197">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Persons with hepatic failure</t>
+          <t>Hospitalization with heart failure events</t>
         </is>
       </c>
       <c r="C197">
-        <v>9999</v>
+        <v>30</v>
       </c>
     </row>
     <row r="198">
       <c r="A198">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Hospitalization with heart failure events</t>
+          <t>Hyperkalemia events</t>
         </is>
       </c>
       <c r="C198">
-        <v>30</v>
+        <v>90</v>
       </c>
     </row>
     <row r="199">
       <c r="A199">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Hyperkalemia events</t>
+          <t>Hypokalemia events</t>
         </is>
       </c>
       <c r="C199">
@@ -2986,11 +2986,11 @@
     </row>
     <row r="200">
       <c r="A200">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Hypokalemia events</t>
+          <t>Hypomagnesemia events</t>
         </is>
       </c>
       <c r="C200">
@@ -2999,37 +2999,37 @@
     </row>
     <row r="201">
       <c r="A201">
-        <v>942</v>
+        <v>956</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Hypomagnesemia events</t>
+          <t>Transient ischemic attack events</t>
         </is>
       </c>
       <c r="C201">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="202">
       <c r="A202">
-        <v>956</v>
+        <v>965</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Transient ischemic attack events</t>
+          <t>3-point MACE</t>
         </is>
       </c>
       <c r="C202">
-        <v>30</v>
+        <v>180</v>
       </c>
     </row>
     <row r="203">
       <c r="A203">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>3-point MACE</t>
+          <t>4-point MACE</t>
         </is>
       </c>
       <c r="C203">
@@ -3038,76 +3038,76 @@
     </row>
     <row r="204">
       <c r="A204">
-        <v>967</v>
+        <v>980</v>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>4-point MACE</t>
+          <t>Coronary Vessel Revascularization</t>
         </is>
       </c>
       <c r="C204">
-        <v>180</v>
+        <v>30</v>
       </c>
     </row>
     <row r="205">
       <c r="A205">
-        <v>980</v>
+        <v>989</v>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Coronary Vessel Revascularization</t>
+          <t>Bladder Cancer</t>
         </is>
       </c>
       <c r="C205">
-        <v>30</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="206">
       <c r="A206">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Bladder Cancer</t>
+          <t>Bone Fracture</t>
         </is>
       </c>
       <c r="C206">
-        <v>9999</v>
+        <v>90</v>
       </c>
     </row>
     <row r="207">
       <c r="A207">
-        <v>990</v>
+        <v>996</v>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Bone Fracture</t>
+          <t>Hypoglycemia</t>
         </is>
       </c>
       <c r="C207">
-        <v>90</v>
+        <v>30</v>
       </c>
     </row>
     <row r="208">
       <c r="A208">
-        <v>996</v>
+        <v>999</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Hypoglycemia</t>
+          <t>Lower extremity amputation</t>
         </is>
       </c>
       <c r="C208">
-        <v>30</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="209">
       <c r="A209">
-        <v>999</v>
+        <v>1003</v>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Lower extremity amputation</t>
+          <t>Renal Cancer</t>
         </is>
       </c>
       <c r="C209">
@@ -3116,11 +3116,11 @@
     </row>
     <row r="210">
       <c r="A210">
-        <v>1003</v>
+        <v>1004</v>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Renal Cancer</t>
+          <t>Thyroid tumor</t>
         </is>
       </c>
       <c r="C210">
@@ -3129,11 +3129,11 @@
     </row>
     <row r="211">
       <c r="A211">
-        <v>1004</v>
+        <v>1007</v>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Thyroid tumor</t>
+          <t>Earliest event of Epilepsy</t>
         </is>
       </c>
       <c r="C211">
@@ -3142,11 +3142,11 @@
     </row>
     <row r="212">
       <c r="A212">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Earliest event of Epilepsy</t>
+          <t>Earliest event of Treatment resistant depression (TRD)</t>
         </is>
       </c>
       <c r="C212">
@@ -3155,11 +3155,11 @@
     </row>
     <row r="213">
       <c r="A213">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Earliest event of Treatment resistant depression (TRD)</t>
+          <t>Earliest event of Chronic Graft Versus Host Disease (GVHD)</t>
         </is>
       </c>
       <c r="C213">
@@ -3168,11 +3168,11 @@
     </row>
     <row r="214">
       <c r="A214">
-        <v>1010</v>
+        <v>1011</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Earliest event of Chronic Graft Versus Host Disease (GVHD)</t>
+          <t>Earliest event of Marginal zone lymphoma</t>
         </is>
       </c>
       <c r="C214">
@@ -3181,11 +3181,11 @@
     </row>
     <row r="215">
       <c r="A215">
-        <v>1011</v>
+        <v>1012</v>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Earliest event of Marginal zone lymphoma</t>
+          <t>Earliest event of Waldenstrom macroglobulinemia</t>
         </is>
       </c>
       <c r="C215">
@@ -3194,11 +3194,11 @@
     </row>
     <row r="216">
       <c r="A216">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Earliest event of Waldenstrom macroglobulinemia</t>
+          <t>Earliest event of Ankylosing Spondylitis</t>
         </is>
       </c>
       <c r="C216">
@@ -3207,11 +3207,11 @@
     </row>
     <row r="217">
       <c r="A217">
-        <v>1013</v>
+        <v>1018</v>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Earliest event of Ankylosing Spondylitis</t>
+          <t>Earliest event of Warm Autoimmune Hemolytic Anemia (wAIHA)</t>
         </is>
       </c>
       <c r="C217">
@@ -3220,11 +3220,11 @@
     </row>
     <row r="218">
       <c r="A218">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Earliest event of Warm Autoimmune Hemolytic Anemia (wAIHA)</t>
+          <t>Earliest event of Major depressive disorder, with NO occurrence of certain psychiatric disorder</t>
         </is>
       </c>
       <c r="C218">
@@ -3233,11 +3233,11 @@
     </row>
     <row r="219">
       <c r="A219">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Earliest event of Major depressive disorder, with NO occurrence of certain psychiatric disorder</t>
+          <t>Earliest event of Myasthenia Gravis, inpatient, 2nd diagnosis or treatment, age gte 18</t>
         </is>
       </c>
       <c r="C219">
@@ -3246,11 +3246,11 @@
     </row>
     <row r="220">
       <c r="A220">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Earliest event of Myasthenia Gravis, inpatient, 2nd diagnosis or treatment, age gte 18</t>
+          <t>Earliest event of Depressive and Sleep Disorder</t>
         </is>
       </c>
       <c r="C220">
@@ -3259,11 +3259,11 @@
     </row>
     <row r="221">
       <c r="A221">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Earliest event of Depressive and Sleep Disorder</t>
+          <t>Earliest Event of Depressive Disorder with Suicidal Ideation or Attempt Prevalent</t>
         </is>
       </c>
       <c r="C221">
@@ -3272,11 +3272,11 @@
     </row>
     <row r="222">
       <c r="A222">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Earliest Event of Depressive Disorder with Suicidal Ideation or Attempt Prevalent</t>
+          <t>Earliest Event of Depressive Disorder with Anhedonia</t>
         </is>
       </c>
       <c r="C222">
@@ -3285,11 +3285,11 @@
     </row>
     <row r="223">
       <c r="A223">
-        <v>1024</v>
+        <v>1025</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Earliest Event of Depressive Disorder with Anhedonia</t>
+          <t>First event of Attention-deficit hyperactivity (ADHD) disorder or procedure</t>
         </is>
       </c>
       <c r="C223">
@@ -3298,11 +3298,11 @@
     </row>
     <row r="224">
       <c r="A224">
-        <v>1025</v>
+        <v>1026</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>First event of Attention-deficit hyperactivity (ADHD) disorder or procedure</t>
+          <t>Earliest Event of Multiple Sclerosis</t>
         </is>
       </c>
       <c r="C224">
@@ -3311,11 +3311,11 @@
     </row>
     <row r="225">
       <c r="A225">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Earliest Event of Multiple Sclerosis</t>
+          <t>Earliest event of Chronic Leukocytic Leukemia</t>
         </is>
       </c>
       <c r="C225">
@@ -3324,11 +3324,11 @@
     </row>
     <row r="226">
       <c r="A226">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Earliest event of Chronic Leukocytic Leukemia</t>
+          <t>Earliest event of Urothelial carcinoma</t>
         </is>
       </c>
       <c r="C226">
@@ -3337,11 +3337,11 @@
     </row>
     <row r="227">
       <c r="A227">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>Earliest event of Urothelial carcinoma</t>
+          <t>Earliest event of Mantle Cell Lymphoma</t>
         </is>
       </c>
       <c r="C227">
@@ -3350,11 +3350,11 @@
     </row>
     <row r="228">
       <c r="A228">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Earliest event of Mantle Cell Lymphoma</t>
+          <t>Earliest event of Prostate cancer, among adult males</t>
         </is>
       </c>
       <c r="C228">
@@ -3363,11 +3363,11 @@
     </row>
     <row r="229">
       <c r="A229">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Earliest event of Prostate cancer, among adult males</t>
+          <t>Earliest event of Coronary artery disease (CAD)</t>
         </is>
       </c>
       <c r="C229">
@@ -3376,11 +3376,11 @@
     </row>
     <row r="230">
       <c r="A230">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Earliest event of Coronary artery disease (CAD)</t>
+          <t>Earliest event of Type 2 Diabetes Mellitus (DM), with no type 1 or secondary DM</t>
         </is>
       </c>
       <c r="C230">
@@ -3389,11 +3389,11 @@
     </row>
     <row r="231">
       <c r="A231">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Earliest event of Type 2 Diabetes Mellitus (DM), with no type 1 or secondary DM</t>
+          <t>Earliest event of Human Immunodeficiency Virus I (HIV), with treatment, lab or 2nd diagnosis</t>
         </is>
       </c>
       <c r="C231">
@@ -3402,50 +3402,50 @@
     </row>
     <row r="232">
       <c r="A232">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Earliest event of Human Immunodeficiency Virus I (HIV), with treatment, lab or 2nd diagnosis</t>
+          <t>All events of Respiratory syncytial virus infection, with 30 days washout</t>
         </is>
       </c>
       <c r="C232">
-        <v>9999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
       <c r="A233">
-        <v>1034</v>
+        <v>1072</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>All events of Respiratory syncytial virus infection, with 30 days washout</t>
+          <t>Cytomegalovirus CMV Anterior Uveitis</t>
         </is>
       </c>
       <c r="C233">
-        <v>0</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="234">
       <c r="A234">
-        <v>1072</v>
+        <v>1073</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Cytomegalovirus CMV Anterior Uveitis</t>
+          <t>Serious Infection, opportunistic infections and other infections of interest event</t>
         </is>
       </c>
       <c r="C234">
-        <v>9999</v>
+        <v>90</v>
       </c>
     </row>
     <row r="235">
       <c r="A235">
-        <v>1073</v>
+        <v>1074</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Serious Infection, opportunistic infections and other infections of interest event</t>
+          <t>Serious Infection</t>
         </is>
       </c>
       <c r="C235">
@@ -3454,50 +3454,50 @@
     </row>
     <row r="236">
       <c r="A236">
-        <v>1074</v>
+        <v>1075</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Serious Infection</t>
+          <t>Narcolepsy</t>
         </is>
       </c>
       <c r="C236">
-        <v>90</v>
+        <v>365</v>
       </c>
     </row>
     <row r="237">
       <c r="A237">
-        <v>1075</v>
+        <v>1076</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Narcolepsy</t>
+          <t>Anaphylaxis</t>
         </is>
       </c>
       <c r="C237">
-        <v>365</v>
+        <v>30</v>
       </c>
     </row>
     <row r="238">
       <c r="A238">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Anaphylaxis</t>
+          <t>Bells Palsy</t>
         </is>
       </c>
       <c r="C238">
-        <v>30</v>
+        <v>183</v>
       </c>
     </row>
     <row r="239">
       <c r="A239">
-        <v>1078</v>
+        <v>1079</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Bells Palsy</t>
+          <t>Encephalomyelitis</t>
         </is>
       </c>
       <c r="C239">
@@ -3506,24 +3506,24 @@
     </row>
     <row r="240">
       <c r="A240">
-        <v>1079</v>
+        <v>1080</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Encephalomyelitis</t>
+          <t>Guillain Barre Syndrome</t>
         </is>
       </c>
       <c r="C240">
-        <v>183</v>
+        <v>365</v>
       </c>
     </row>
     <row r="241">
       <c r="A241">
-        <v>1080</v>
+        <v>1081</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Guillain Barre Syndrome</t>
+          <t>Acute Myocardial Infarction including its complications</t>
         </is>
       </c>
       <c r="C241">
@@ -3532,11 +3532,11 @@
     </row>
     <row r="242">
       <c r="A242">
-        <v>1081</v>
+        <v>1082</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Acute Myocardial Infarction including its complications</t>
+          <t>Myocarditis Pericarditis</t>
         </is>
       </c>
       <c r="C242">
@@ -3545,11 +3545,11 @@
     </row>
     <row r="243">
       <c r="A243">
-        <v>1082</v>
+        <v>1083</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Myocarditis Pericarditis</t>
+          <t>Immune Thrombocytopenia (ITP)</t>
         </is>
       </c>
       <c r="C243">
@@ -3558,11 +3558,11 @@
     </row>
     <row r="244">
       <c r="A244">
-        <v>1083</v>
+        <v>1084</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Immune Thrombocytopenia (ITP)</t>
+          <t>Disseminated Intravascular Coagulation</t>
         </is>
       </c>
       <c r="C244">
@@ -3571,11 +3571,11 @@
     </row>
     <row r="245">
       <c r="A245">
-        <v>1084</v>
+        <v>1087</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Disseminated Intravascular Coagulation</t>
+          <t>Hemorrhagic Stroke</t>
         </is>
       </c>
       <c r="C245">
@@ -3584,11 +3584,11 @@
     </row>
     <row r="246">
       <c r="A246">
-        <v>1087</v>
+        <v>1088</v>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Hemorrhagic Stroke</t>
+          <t>Deep Vein Thrombosis (DVT)</t>
         </is>
       </c>
       <c r="C246">
@@ -3597,11 +3597,11 @@
     </row>
     <row r="247">
       <c r="A247">
-        <v>1088</v>
+        <v>1089</v>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>Deep Vein Thrombosis (DVT)</t>
+          <t>Non-hemorrhagic Stroke</t>
         </is>
       </c>
       <c r="C247">
@@ -3610,11 +3610,11 @@
     </row>
     <row r="248">
       <c r="A248">
-        <v>1089</v>
+        <v>1090</v>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Non-hemorrhagic Stroke</t>
+          <t>Pulmonary Embolism</t>
         </is>
       </c>
       <c r="C248">
@@ -3623,11 +3623,11 @@
     </row>
     <row r="249">
       <c r="A249">
-        <v>1090</v>
+        <v>1091</v>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>Pulmonary Embolism</t>
+          <t>Thrombosis with Thrombocytopenia (TWT)</t>
         </is>
       </c>
       <c r="C249">
@@ -3636,24 +3636,24 @@
     </row>
     <row r="250">
       <c r="A250">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Thrombosis with Thrombocytopenia (TWT)</t>
+          <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C250">
-        <v>365</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="251">
       <c r="A251">
-        <v>1093</v>
+        <v>1094</v>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>Abdominal Aoritc Aneurysm repair - post op new Afib (any)</t>
+          <t>Lower Extremity Bypass - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C251">
@@ -3662,11 +3662,11 @@
     </row>
     <row r="252">
       <c r="A252">
-        <v>1094</v>
+        <v>1095</v>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Lower Extremity Bypass - post op new Afib (any)</t>
+          <t>Carotid Endarterectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C252">
@@ -3675,11 +3675,11 @@
     </row>
     <row r="253">
       <c r="A253">
-        <v>1095</v>
+        <v>1096</v>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>Carotid Endarterectomy - post op new Afib (any)</t>
+          <t>Lung Resection - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C253">
@@ -3688,11 +3688,11 @@
     </row>
     <row r="254">
       <c r="A254">
-        <v>1096</v>
+        <v>1097</v>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>Lung Resection - post op new Afib (any)</t>
+          <t>Esophagectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C254">
@@ -3701,11 +3701,11 @@
     </row>
     <row r="255">
       <c r="A255">
-        <v>1097</v>
+        <v>1098</v>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>Esophagectomy - post op new Afib (any)</t>
+          <t>Pancreatectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C255">
@@ -3714,11 +3714,11 @@
     </row>
     <row r="256">
       <c r="A256">
-        <v>1098</v>
+        <v>1099</v>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Pancreatectomy - post op new Afib (any)</t>
+          <t>Colectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C256">
@@ -3727,11 +3727,11 @@
     </row>
     <row r="257">
       <c r="A257">
-        <v>1099</v>
+        <v>1100</v>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>Colectomy - post op new Afib (any)</t>
+          <t>Cystectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C257">
@@ -3740,11 +3740,11 @@
     </row>
     <row r="258">
       <c r="A258">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>Cystectomy - post op new Afib (any)</t>
+          <t>Nephrectomy - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C258">
@@ -3753,11 +3753,11 @@
     </row>
     <row r="259">
       <c r="A259">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>Nephrectomy - post op new Afib (any)</t>
+          <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C259">
@@ -3766,11 +3766,11 @@
     </row>
     <row r="260">
       <c r="A260">
-        <v>1102</v>
+        <v>1103</v>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>Coronary Artery Bypass Graft Surgery - post op new Afib (any)</t>
+          <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
         </is>
       </c>
       <c r="C260">
@@ -3779,37 +3779,37 @@
     </row>
     <row r="261">
       <c r="A261">
-        <v>1103</v>
+        <v>1104</v>
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>Aortic or Mitral Valve Repair or Replacement - post op new Afib (any)</t>
+          <t>RBC Transfusion (adult relevant, no auto 1yr clean window)</t>
         </is>
       </c>
       <c r="C261">
-        <v>9999</v>
+        <v>30</v>
       </c>
     </row>
     <row r="262">
       <c r="A262">
-        <v>1104</v>
+        <v>1105</v>
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>RBC Transfusion (adult relevant, no auto 1yr clean window)</t>
+          <t>Clostridium difficile - first episode</t>
         </is>
       </c>
       <c r="C262">
-        <v>30</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="263">
       <c r="A263">
-        <v>1105</v>
+        <v>1106</v>
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>Clostridium difficile - first episode</t>
+          <t>Non-Emergent Major Non Cardiac Surgery no prior Opioid</t>
         </is>
       </c>
       <c r="C263">
@@ -3818,11 +3818,11 @@
     </row>
     <row r="264">
       <c r="A264">
-        <v>1106</v>
+        <v>1150</v>
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>Non-Emergent Major Non Cardiac Surgery no prior Opioid</t>
+          <t>Emergency room visits (0Pe, 0Era)</t>
         </is>
       </c>
       <c r="C264">
@@ -3831,27 +3831,14 @@
     </row>
     <row r="265">
       <c r="A265">
-        <v>1150</v>
+        <v>1151</v>
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>Emergency room visits (0Pe, 0Era)</t>
+          <t>Autism</t>
         </is>
       </c>
       <c r="C265">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266">
-        <v>1151</v>
-      </c>
-      <c r="B266" t="inlineStr">
-        <is>
-          <t>Autism</t>
-        </is>
-      </c>
-      <c r="C266">
         <v>9999</v>
       </c>
     </row>

</xml_diff>